<commit_message>
New version and release
</commit_message>
<xml_diff>
--- a/requirements/ModelCatalogRequirements.xlsx
+++ b/requirements/ModelCatalogRequirements.xlsx
@@ -18,7 +18,6 @@
     <sheet name="June 2019 (v1.0.0)" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -35,6 +34,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Thanks for starting this document. For the requirements, I think the main driver must be the competency question, which you have placed under this column. I think that we should just have a list of competency questions, and then explain how we have addressed them. Almost like you have done, but with a little reorganization
 	-Daniel Garijo
@@ -63,6 +63,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Not clear what the range is in some of these.
 	-Daniel Garijo
@@ -84,6 +85,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Sorry, your comments disappeared +dgarijo@isi.edu. I think "variable" is in the commons ontology right? But yes, I agree we should name is variable presentation. 
 And I know that some of these are already in the model. I was just trying to get everything in one place if we're going to add a rationale as well (for some reason, I know this is coming)
@@ -106,6 +108,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>We are capturing this through the dataset specification. Configuration - hasInput-&gt; DatasetSpecification-hasFormat-&gt;F.
 	-Daniel Garijo</t>
@@ -119,6 +122,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Units cannot be a string, otherwise we cannot do automatic unit transformation (at the moment it is that way for simplicity). We need to adopt Jay's standard
 	-Daniel Garijo
@@ -134,6 +138,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>JSON file? It would make sense to have a collection of variables, right? Or an entity called "CAG". To be defined
 	-Daniel Garijo
@@ -149,6 +154,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>This one we have to think it in detail. It may be more than this
 	-Daniel Garijo
@@ -164,6 +170,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>In the slides, Yolanda was mentioning queries such as the variables associated to a process. Are we also going to represent these?
 	-Daniel Garijo
@@ -189,6 +196,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>+dgarijo@isi.edu This would be much easier the other way around where the variables would be assign a column number much like what we did in LinkedEarth
 	-Deborah Khider
@@ -210,6 +218,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>+dgarijo@isi.edu This is probably going to be part of the DatasetSpecification Schema
 	-Deborah Khider</t>
@@ -223,6 +232,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>@dgarijo Not sure what the CAG class would look like. It's really a JSON file
 	-Deborah Khider</t>
@@ -234,7 +244,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="331">
   <si>
     <t>What?</t>
   </si>
@@ -1136,9 +1146,6 @@
     <t>Needed for reference</t>
   </si>
   <si>
-    <t>sdm:Calibration, sdm:calibrationMethod, xsd:string</t>
-  </si>
-  <si>
     <t>To be expanded in a future version of the ontology</t>
   </si>
   <si>
@@ -1155,9 +1162,6 @@
   </si>
   <si>
     <t>Which variables can you adjust (if any) on a calibration?</t>
-  </si>
-  <si>
-    <t>sdm:Calibration, sdm:adjustableVariable, sd:VariablePresentation</t>
   </si>
   <si>
     <t>sdm:Model, sd:hasVersion,sd:SoftwareVersion</t>
@@ -1193,9 +1197,6 @@
     <t>sdm:ModelConfiguration, sdm:calibratedVariable, sd:VariablePresentation</t>
   </si>
   <si>
-    <t>sdm:Calibration, sdm:calibrationTargetVariable, sd:VariablePresentation</t>
-  </si>
-  <si>
     <t>sdm:ModelConfiguration, sdm:parameterAssignment, xsd:string</t>
   </si>
   <si>
@@ -1219,6 +1220,27 @@
   <si>
     <t>Needed for the calibrations of a model, in order to describe them transparently</t>
   </si>
+  <si>
+    <t>sdm:ModelConfiguration, sdm:ModelConfigurationTargetVariable, sd:VariablePresentation</t>
+  </si>
+  <si>
+    <t>sdm:ModelConfiguration, sdm:ModelConfigurationMethod, xsd:string</t>
+  </si>
+  <si>
+    <t>sdm:ModelConfiguration, sdm:adjustableVariable, sd:VariablePresentation</t>
+  </si>
+  <si>
+    <t>Is this model calibration still valid?</t>
+  </si>
+  <si>
+    <t>What temporal coverage was this model calibrated with?</t>
+  </si>
+  <si>
+    <t>sdm:validUntil</t>
+  </si>
+  <si>
+    <t>sdm:calibrationInterval</t>
+  </si>
 </sst>
 </file>
 
@@ -1233,11 +1255,13 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1394,7 +1418,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1566,6 +1590,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -60521,8 +60548,8 @@
   </sheetPr>
   <dimension ref="A1:E1252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -60570,7 +60597,7 @@
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="str">
-        <f t="shared" ref="A3:A51" si="0">CONCATENATE("CQ",ROW(A3)-2)</f>
+        <f t="shared" ref="A3:A53" si="0">CONCATENATE("CQ",ROW(A3)-2)</f>
         <v>CQ1</v>
       </c>
       <c r="B3" s="23" t="s">
@@ -60580,7 +60607,7 @@
         <v>29</v>
       </c>
       <c r="D3" s="58" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E3" s="23" t="s">
         <v>245</v>
@@ -60810,7 +60837,7 @@
         <v>143</v>
       </c>
       <c r="D16" s="58" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E16" s="23"/>
     </row>
@@ -60826,7 +60853,7 @@
         <v>265</v>
       </c>
       <c r="D17" s="58" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E17" s="23"/>
     </row>
@@ -60842,7 +60869,7 @@
         <v>264</v>
       </c>
       <c r="D18" s="58" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E18" s="23"/>
     </row>
@@ -60980,7 +61007,7 @@
         <v>179</v>
       </c>
       <c r="D26" s="58" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E26" s="23" t="s">
         <v>245</v>
@@ -60998,7 +61025,7 @@
         <v>185</v>
       </c>
       <c r="D27" s="58" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="E27" s="23" t="s">
         <v>245</v>
@@ -61064,7 +61091,7 @@
         <v>200</v>
       </c>
       <c r="D31" s="58" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E31" s="26"/>
     </row>
@@ -61134,7 +61161,7 @@
         <v>281</v>
       </c>
       <c r="D35" s="58" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E35" s="26"/>
     </row>
@@ -61162,7 +61189,7 @@
       </c>
       <c r="C37" s="26"/>
       <c r="D37" s="58" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E37" s="26"/>
     </row>
@@ -61194,7 +61221,7 @@
       </c>
       <c r="C39" s="26"/>
       <c r="D39" s="58" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E39" s="26"/>
     </row>
@@ -61210,7 +61237,7 @@
         <v>286</v>
       </c>
       <c r="D40" s="58" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E40" s="26"/>
     </row>
@@ -61272,7 +61299,7 @@
         <v>296</v>
       </c>
       <c r="D44" s="58" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E44" s="26"/>
     </row>
@@ -61288,7 +61315,7 @@
         <v>295</v>
       </c>
       <c r="D45" s="58" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="E45" s="26"/>
     </row>
@@ -61304,10 +61331,10 @@
         <v>298</v>
       </c>
       <c r="D46" s="58" t="s">
-        <v>299</v>
+        <v>325</v>
       </c>
       <c r="E46" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="40" customFormat="1" ht="28.8" x14ac:dyDescent="0.25">
@@ -61316,13 +61343,13 @@
         <v>CQ45</v>
       </c>
       <c r="B47" s="55" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C47" s="55" t="s">
         <v>294</v>
       </c>
       <c r="D47" s="59" t="s">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="E47" s="55"/>
     </row>
@@ -61332,13 +61359,13 @@
         <v>CQ46</v>
       </c>
       <c r="B48" s="56" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C48" s="57" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D48" s="60" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="E48" s="57"/>
     </row>
@@ -61348,11 +61375,11 @@
         <v>CQ47</v>
       </c>
       <c r="B49" s="57" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C49" s="57"/>
       <c r="D49" s="60" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="E49" s="57"/>
     </row>
@@ -61362,13 +61389,13 @@
         <v>CQ48</v>
       </c>
       <c r="B50" s="57" t="s">
+        <v>302</v>
+      </c>
+      <c r="C50" s="57" t="s">
         <v>303</v>
       </c>
-      <c r="C50" s="57" t="s">
-        <v>304</v>
-      </c>
       <c r="D50" s="60" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="E50" s="57"/>
     </row>
@@ -61378,21 +61405,39 @@
         <v>CQ49</v>
       </c>
       <c r="B51" s="57" t="s">
+        <v>320</v>
+      </c>
+      <c r="C51" s="57" t="s">
         <v>323</v>
       </c>
-      <c r="C51" s="57" t="s">
-        <v>326</v>
-      </c>
       <c r="D51" s="57" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="E51" s="57"/>
     </row>
-    <row r="52" spans="1:5" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="47"/>
-    </row>
-    <row r="53" spans="1:5" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="47"/>
+    <row r="52" spans="1:5" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="56" t="str">
+        <f t="shared" si="0"/>
+        <v>CQ50</v>
+      </c>
+      <c r="B52" s="63" t="s">
+        <v>327</v>
+      </c>
+      <c r="D52" s="65" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="56" t="str">
+        <f t="shared" si="0"/>
+        <v>CQ51</v>
+      </c>
+      <c r="B53" s="64" t="s">
+        <v>328</v>
+      </c>
+      <c r="D53" s="65" t="s">
+        <v>330</v>
+      </c>
     </row>
     <row r="54" spans="1:5" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="47"/>

</xml_diff>